<commit_message>
add treatments to group parser, in progress
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/group_report_template.xlsx
+++ b/bio_diversity/static/report_templates/group_report_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Event History" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Individual Report:</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Program:</t>
+  </si>
+  <si>
+    <t>Treatments</t>
+  </si>
+  <si>
+    <t>Treatment</t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -566,9 +572,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -576,14 +582,20 @@
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -595,6 +607,15 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix env treatments on group and individual reports, #813
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/group_report_template.xlsx
+++ b/bio_diversity/static/report_templates/group_report_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Individual Report:</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Treatment</t>
+  </si>
+  <si>
+    <t>Duration (mins)</t>
+  </si>
+  <si>
+    <t>Concentration</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -572,22 +581,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -595,7 +607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -616,6 +628,15 @@
       </c>
       <c r="I4" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>